<commit_message>
[ADD] TDSQL OUTPUT DRIVER 新增TDSQL导出驱动
</commit_message>
<xml_diff>
--- a/release/table-data-format-transform-app/output_dataset/output_test.xlsx
+++ b/release/table-data-format-transform-app/output_dataset/output_test.xlsx
@@ -466,10 +466,8 @@
           <t>2003</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1233</t>
-        </is>
+      <c r="C2" t="n">
+        <v>1233</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -488,10 +486,8 @@
           <t>2005</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2343</t>
-        </is>
+      <c r="C3" t="n">
+        <v>2343</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -510,10 +506,8 @@
           <t>2004</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3212</t>
-        </is>
+      <c r="C4" t="n">
+        <v>3212</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -532,10 +526,8 @@
           <t>2003</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1233</t>
-        </is>
+      <c r="C5" t="n">
+        <v>1233</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -554,10 +546,8 @@
           <t>2005</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2343</t>
-        </is>
+      <c r="C6" t="n">
+        <v>2343</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -576,10 +566,8 @@
           <t>2004</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>3212</t>
-        </is>
+      <c r="C7" t="n">
+        <v>3212</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>

</xml_diff>